<commit_message>
deploy: add startup commands
</commit_message>
<xml_diff>
--- a/deploy.xlsx
+++ b/deploy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shun.cheung/Documents/learning/casualapp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29843860-BCDC-474D-A032-0ECA01ADB860}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFCB23DC-4A68-7C47-813B-BE965EF60912}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="100" yWindow="460" windowWidth="24020" windowHeight="17540" xr2:uid="{D70ABF78-F301-B84D-BD2E-246F7AB1B5AF}"/>
+    <workbookView xWindow="4780" yWindow="460" windowWidth="24020" windowHeight="17540" xr2:uid="{D70ABF78-F301-B84D-BD2E-246F7AB1B5AF}"/>
   </bookViews>
   <sheets>
     <sheet name="application deploy commands" sheetId="13" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="59">
   <si>
     <t>Python</t>
   </si>
@@ -202,6 +202,9 @@
   </si>
   <si>
     <t>20190925-01</t>
+  </si>
+  <si>
+    <t>celery flower -A backend --port=5555 -f /var/log/casualapp/flower.log &amp;</t>
   </si>
 </sst>
 </file>
@@ -326,7 +329,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -346,7 +349,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -668,10 +670,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{895829AB-853F-4A40-A4D0-66E43545364D}">
-  <dimension ref="A2:F61"/>
+  <dimension ref="A2:F62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42:D44"/>
+    <sheetView tabSelected="1" topLeftCell="B23" workbookViewId="0">
+      <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -685,41 +687,41 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
       <c r="D2" s="2"/>
     </row>
     <row r="3" spans="1:6" ht="19">
       <c r="A3" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="C3" s="16"/>
+      <c r="C3" s="15"/>
       <c r="D3" s="2"/>
     </row>
     <row r="4" spans="1:6" ht="19">
       <c r="A4" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="C4" s="16"/>
+      <c r="C4" s="15"/>
       <c r="D4" s="2"/>
     </row>
     <row r="5" spans="1:6" ht="19">
       <c r="A5" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="C5" s="16"/>
+      <c r="C5" s="15"/>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="5"/>
@@ -1114,71 +1116,74 @@
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="2"/>
-      <c r="C52" s="2" t="s">
+      <c r="C52" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="C53" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="C54" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D54" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="E54" s="2"/>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="C56" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="D52" s="2" t="s">
+      <c r="D56" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="E52" s="2"/>
-    </row>
-    <row r="53" spans="1:5">
-      <c r="B53" s="2"/>
-      <c r="C53" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D53" s="2" t="s">
+    </row>
+    <row r="57" spans="1:5">
+      <c r="C57" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="D57" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="E53" s="2"/>
-    </row>
-    <row r="54" spans="1:5">
-      <c r="C54" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D54" s="2" t="s">
+    </row>
+    <row r="58" spans="1:5">
+      <c r="C58" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="D58" s="13" t="s">
         <v>53</v>
-      </c>
-      <c r="E54" s="2"/>
-    </row>
-    <row r="55" spans="1:5">
-      <c r="C55" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5">
-      <c r="C58" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="D58" s="14" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="59" spans="1:5">
       <c r="C59" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="D59" s="14" t="s">
-        <v>51</v>
+      <c r="D59" s="13" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="60" spans="1:5">
-      <c r="C60" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="D60" s="14" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5">
-      <c r="C61" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="D61" s="13" t="s">
-        <v>24</v>
+      <c r="C60" s="13"/>
+      <c r="D60" s="13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="C62" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="D62" s="13" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
deploy: path to startup
</commit_message>
<xml_diff>
--- a/deploy.xlsx
+++ b/deploy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shun.cheung/Documents/learning/casualapp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFCB23DC-4A68-7C47-813B-BE965EF60912}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EE2BF4A-D4FF-A747-9186-22C455ED7677}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4780" yWindow="460" windowWidth="24020" windowHeight="17540" xr2:uid="{D70ABF78-F301-B84D-BD2E-246F7AB1B5AF}"/>
   </bookViews>
@@ -183,9 +183,6 @@
     <t>cd /usr/local/casualapp/active</t>
   </si>
   <si>
-    <t>sh /usr/local/casualapp/startup.sh</t>
-  </si>
-  <si>
     <t>uwsgi --restart /usr/local/casualapp/active/casualapp.pid</t>
   </si>
   <si>
@@ -201,10 +198,13 @@
     <t xml:space="preserve">pkill -9 celery </t>
   </si>
   <si>
-    <t>20190925-01</t>
-  </si>
-  <si>
     <t>celery flower -A backend --port=5555 -f /var/log/casualapp/flower.log &amp;</t>
+  </si>
+  <si>
+    <t>20190928-01</t>
+  </si>
+  <si>
+    <t>sh /usr/local/casualapp/active/startup.sh</t>
   </si>
 </sst>
 </file>
@@ -672,8 +672,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{895829AB-853F-4A40-A4D0-66E43545364D}">
   <dimension ref="A2:F62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B23" workbookViewId="0">
-      <selection activeCell="C51" sqref="C51"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -801,7 +801,7 @@
       </c>
       <c r="D13" t="str">
         <f xml:space="preserve"> "cp -r backend " &amp; $B$4</f>
-        <v>cp -r backend 20190925-01</v>
+        <v>cp -r backend 20190928-01</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -819,7 +819,7 @@
       </c>
       <c r="D15" t="str">
         <f>"touch "&amp;$B$5&amp;"/" &amp; $B$4&amp; "/base/static/empty.txt &amp;&amp; rm -r "&amp;$B$5&amp;"/" &amp; $B$4&amp; "/base/static/* &amp;&amp; rsync -av " &amp; $B$5 &amp;"/frontend/build/index.html "&amp;$B$5&amp;"/" &amp; $B$4&amp; "/base/templates/. &amp;&amp; rsync -av --exclude='static' "  &amp; $B$5 &amp;"/frontend/build/* "&amp; $B$5 &amp;"/" &amp; $B$4&amp; "/base/static/. &amp;&amp; rsync -av " &amp; $B$5 &amp;"/frontend/build/static/* "&amp;$B$5&amp;"/" &amp; $B$4&amp; "/base/static/."</f>
-        <v>touch /Users/shun.cheung/Documents/learning/casualapp/20190925-01/base/static/empty.txt &amp;&amp; rm -r /Users/shun.cheung/Documents/learning/casualapp/20190925-01/base/static/* &amp;&amp; rsync -av /Users/shun.cheung/Documents/learning/casualapp/frontend/build/index.html /Users/shun.cheung/Documents/learning/casualapp/20190925-01/base/templates/. &amp;&amp; rsync -av --exclude='static' /Users/shun.cheung/Documents/learning/casualapp/frontend/build/* /Users/shun.cheung/Documents/learning/casualapp/20190925-01/base/static/. &amp;&amp; rsync -av /Users/shun.cheung/Documents/learning/casualapp/frontend/build/static/* /Users/shun.cheung/Documents/learning/casualapp/20190925-01/base/static/.</v>
+        <v>touch /Users/shun.cheung/Documents/learning/casualapp/20190928-01/base/static/empty.txt &amp;&amp; rm -r /Users/shun.cheung/Documents/learning/casualapp/20190928-01/base/static/* &amp;&amp; rsync -av /Users/shun.cheung/Documents/learning/casualapp/frontend/build/index.html /Users/shun.cheung/Documents/learning/casualapp/20190928-01/base/templates/. &amp;&amp; rsync -av --exclude='static' /Users/shun.cheung/Documents/learning/casualapp/frontend/build/* /Users/shun.cheung/Documents/learning/casualapp/20190928-01/base/static/. &amp;&amp; rsync -av /Users/shun.cheung/Documents/learning/casualapp/frontend/build/static/* /Users/shun.cheung/Documents/learning/casualapp/20190928-01/base/static/.</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -837,7 +837,7 @@
       </c>
       <c r="D17" t="str">
         <f>"pip freeze &gt; "&amp;$B$5 &amp;"/"&amp;$B$4&amp;"/requirement.txt"</f>
-        <v>pip freeze &gt; /Users/shun.cheung/Documents/learning/casualapp/20190925-01/requirement.txt</v>
+        <v>pip freeze &gt; /Users/shun.cheung/Documents/learning/casualapp/20190928-01/requirement.txt</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -846,7 +846,7 @@
       </c>
       <c r="D18" t="str">
         <f>"python "&amp;$B$5&amp;"/"&amp;$B$4&amp;"/manage.py collectstatic"</f>
-        <v>python /Users/shun.cheung/Documents/learning/casualapp/20190925-01/manage.py collectstatic</v>
+        <v>python /Users/shun.cheung/Documents/learning/casualapp/20190928-01/manage.py collectstatic</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -863,7 +863,7 @@
       </c>
       <c r="D21" t="str">
         <f>"vi "&amp;$B$5&amp;"/"&amp;$B$4&amp;"/backend/settings.py"</f>
-        <v>vi /Users/shun.cheung/Documents/learning/casualapp/20190925-01/backend/settings.py</v>
+        <v>vi /Users/shun.cheung/Documents/learning/casualapp/20190928-01/backend/settings.py</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="15" customHeight="1"/>
@@ -882,7 +882,7 @@
       </c>
       <c r="D24" t="str">
         <f>"zip -r "&amp;$B$4&amp;".zip "&amp;$B$4</f>
-        <v>zip -r 20190925-01.zip 20190925-01</v>
+        <v>zip -r 20190928-01.zip 20190928-01</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -891,7 +891,7 @@
       </c>
       <c r="D25" t="str">
         <f>"rm -r "&amp;B4</f>
-        <v>rm -r 20190925-01</v>
+        <v>rm -r 20190928-01</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -926,7 +926,7 @@
       </c>
       <c r="D30" t="str">
         <f>"put "&amp;B4&amp;".zip"</f>
-        <v>put 20190925-01.zip</v>
+        <v>put 20190928-01.zip</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -943,7 +943,7 @@
       </c>
       <c r="D33" t="str">
         <f>"rm -r "&amp;B4 &amp; ".zip"</f>
-        <v>rm -r 20190925-01.zip</v>
+        <v>rm -r 20190928-01.zip</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -966,7 +966,7 @@
       </c>
       <c r="D36" t="str">
         <f>"mv " &amp; $B$4 &amp;".zip /usr/local/casualapp/"</f>
-        <v>mv 20190925-01.zip /usr/local/casualapp/</v>
+        <v>mv 20190928-01.zip /usr/local/casualapp/</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -983,7 +983,7 @@
       </c>
       <c r="D38" t="str">
         <f>"unzip /usr/local/casualapp/"&amp;$B$4&amp;".zip -d ."</f>
-        <v>unzip /usr/local/casualapp/20190925-01.zip -d .</v>
+        <v>unzip /usr/local/casualapp/20190928-01.zip -d .</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -995,7 +995,7 @@
       </c>
       <c r="D39" t="str">
         <f>"ln -sfn /usr/local/casualapp/"&amp;$B$4&amp;" /usr/local/casualapp/active"</f>
-        <v>ln -sfn /usr/local/casualapp/20190925-01 /usr/local/casualapp/active</v>
+        <v>ln -sfn /usr/local/casualapp/20190928-01 /usr/local/casualapp/active</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -1021,7 +1021,7 @@
         <v>29</v>
       </c>
       <c r="D42" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E42" s="2"/>
     </row>
@@ -1030,7 +1030,7 @@
         <v>29</v>
       </c>
       <c r="D43" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E43" s="12" t="s">
         <v>36</v>
@@ -1120,7 +1120,7 @@
         <v>29</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
     </row>
     <row r="53" spans="1:5">
@@ -1161,7 +1161,7 @@
         <v>29</v>
       </c>
       <c r="D58" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="59" spans="1:5">
@@ -1169,13 +1169,13 @@
         <v>29</v>
       </c>
       <c r="D59" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="60" spans="1:5">
       <c r="C60" s="13"/>
       <c r="D60" s="13" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="62" spans="1:5">
@@ -1183,7 +1183,7 @@
         <v>29</v>
       </c>
       <c r="D62" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>